<commit_message>
Dataset cleaned, now make the interactive graphs on C#
</commit_message>
<xml_diff>
--- a/Datasets/Texas COVID-19 New Confirmed Cases by County.xlsx
+++ b/Datasets/Texas COVID-19 New Confirmed Cases by County.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Academical Things\Programming\R\Workspaces\SE_project\Datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{046306BA-1B51-44F6-855E-25F4B1718E56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1ACB84D0-B7E6-4D62-9429-8B535B4E9AD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="New Cases by County 2020" sheetId="1" r:id="rId1"/>
@@ -1539,9 +1539,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="mm/dd/yyyy"/>
-  </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1605,18 +1602,22 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -1959,9 +1960,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:KP2"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1970,8 +1969,8 @@
     <col min="303" max="309" width="9.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:302" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:302" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3">
@@ -3797,7 +3796,7 @@
   <dimension ref="A1:NB261"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -3812,8 +3811,8 @@
     <col min="367" max="371" width="9.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:366" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:366" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3">
@@ -6280,8 +6279,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:NB2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6292,1102 +6291,1102 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:366" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="J1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="K1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="L1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="M1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="N1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="O1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="P1" s="4" t="s">
+      <c r="P1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="Q1" s="4" t="s">
+      <c r="Q1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="R1" s="4" t="s">
+      <c r="R1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="S1" s="4" t="s">
+      <c r="S1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="T1" s="4" t="s">
+      <c r="T1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="U1" s="4" t="s">
+      <c r="U1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="V1" s="4" t="s">
+      <c r="V1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="W1" s="4" t="s">
+      <c r="W1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="X1" s="4" t="s">
+      <c r="X1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="Y1" s="4" t="s">
+      <c r="Y1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="Z1" s="4" t="s">
+      <c r="Z1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="AA1" s="4" t="s">
+      <c r="AA1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="AB1" s="4" t="s">
+      <c r="AB1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="AC1" s="4" t="s">
+      <c r="AC1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="AD1" s="4" t="s">
+      <c r="AD1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="AE1" s="4" t="s">
+      <c r="AE1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="AF1" s="4" t="s">
+      <c r="AF1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="AG1" s="4" t="s">
+      <c r="AG1" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="AH1" s="4" t="s">
+      <c r="AH1" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="AI1" s="4" t="s">
+      <c r="AI1" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="AJ1" s="4" t="s">
+      <c r="AJ1" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="AK1" s="4" t="s">
+      <c r="AK1" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="AL1" s="4" t="s">
+      <c r="AL1" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="AM1" s="4" t="s">
+      <c r="AM1" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="AN1" s="4" t="s">
+      <c r="AN1" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AO1" s="4" t="s">
+      <c r="AO1" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="AP1" s="4" t="s">
+      <c r="AP1" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="AQ1" s="4" t="s">
+      <c r="AQ1" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="AR1" s="4" t="s">
+      <c r="AR1" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="AS1" s="4" t="s">
+      <c r="AS1" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="AT1" s="4" t="s">
+      <c r="AT1" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="AU1" s="4" t="s">
+      <c r="AU1" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="AV1" s="4" t="s">
+      <c r="AV1" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="AW1" s="4" t="s">
+      <c r="AW1" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="AX1" s="4" t="s">
+      <c r="AX1" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="AY1" s="4" t="s">
+      <c r="AY1" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="AZ1" s="4" t="s">
+      <c r="AZ1" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="BA1" s="4" t="s">
+      <c r="BA1" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="BB1" s="4" t="s">
+      <c r="BB1" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="BC1" s="4" t="s">
+      <c r="BC1" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="BD1" s="4" t="s">
+      <c r="BD1" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="BE1" s="4" t="s">
+      <c r="BE1" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="BF1" s="4" t="s">
+      <c r="BF1" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="BG1" s="4" t="s">
+      <c r="BG1" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="BH1" s="4" t="s">
+      <c r="BH1" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="BI1" s="4" t="s">
+      <c r="BI1" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="BJ1" s="4" t="s">
+      <c r="BJ1" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="BK1" s="4" t="s">
+      <c r="BK1" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="BL1" s="4" t="s">
+      <c r="BL1" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="BM1" s="4" t="s">
+      <c r="BM1" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="BN1" s="4" t="s">
+      <c r="BN1" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="BO1" s="4" t="s">
+      <c r="BO1" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="BP1" s="4" t="s">
+      <c r="BP1" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="BQ1" s="4" t="s">
+      <c r="BQ1" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="BR1" s="4" t="s">
+      <c r="BR1" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="BS1" s="4" t="s">
+      <c r="BS1" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="BT1" s="4" t="s">
+      <c r="BT1" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="BU1" s="4" t="s">
+      <c r="BU1" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="BV1" s="4" t="s">
+      <c r="BV1" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="BW1" s="4" t="s">
+      <c r="BW1" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="BX1" s="4" t="s">
+      <c r="BX1" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="BY1" s="4" t="s">
+      <c r="BY1" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="BZ1" s="4" t="s">
+      <c r="BZ1" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="CA1" s="4" t="s">
+      <c r="CA1" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="CB1" s="4" t="s">
+      <c r="CB1" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="CC1" s="4" t="s">
+      <c r="CC1" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="CD1" s="4" t="s">
+      <c r="CD1" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="CE1" s="4" t="s">
+      <c r="CE1" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="CF1" s="4" t="s">
+      <c r="CF1" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="CG1" s="4" t="s">
+      <c r="CG1" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="CH1" s="4" t="s">
+      <c r="CH1" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="CI1" s="4" t="s">
+      <c r="CI1" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="CJ1" s="4" t="s">
+      <c r="CJ1" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="CK1" s="4" t="s">
+      <c r="CK1" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="CL1" s="4" t="s">
+      <c r="CL1" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="CM1" s="4" t="s">
+      <c r="CM1" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="CN1" s="4" t="s">
+      <c r="CN1" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="CO1" s="4" t="s">
+      <c r="CO1" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="CP1" s="4" t="s">
+      <c r="CP1" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="CQ1" s="4" t="s">
+      <c r="CQ1" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="CR1" s="4" t="s">
+      <c r="CR1" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="CS1" s="4" t="s">
+      <c r="CS1" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="CT1" s="4" t="s">
+      <c r="CT1" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="CU1" s="4" t="s">
+      <c r="CU1" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="CV1" s="4" t="s">
+      <c r="CV1" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="CW1" s="4" t="s">
+      <c r="CW1" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="CX1" s="4" t="s">
+      <c r="CX1" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="CY1" s="4" t="s">
+      <c r="CY1" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="CZ1" s="4" t="s">
+      <c r="CZ1" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="DA1" s="4" t="s">
+      <c r="DA1" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="DB1" s="4" t="s">
+      <c r="DB1" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="DC1" s="4" t="s">
+      <c r="DC1" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="DD1" s="4" t="s">
+      <c r="DD1" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="DE1" s="4" t="s">
+      <c r="DE1" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="DF1" s="4" t="s">
+      <c r="DF1" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="DG1" s="4" t="s">
+      <c r="DG1" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="DH1" s="4" t="s">
+      <c r="DH1" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="DI1" s="4" t="s">
+      <c r="DI1" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="DJ1" s="4" t="s">
+      <c r="DJ1" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="DK1" s="4" t="s">
+      <c r="DK1" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="DL1" s="4" t="s">
+      <c r="DL1" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="DM1" s="4" t="s">
+      <c r="DM1" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="DN1" s="4" t="s">
+      <c r="DN1" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="DO1" s="4" t="s">
+      <c r="DO1" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="DP1" s="4" t="s">
+      <c r="DP1" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="DQ1" s="4" t="s">
+      <c r="DQ1" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="DR1" s="4" t="s">
+      <c r="DR1" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="DS1" s="4" t="s">
+      <c r="DS1" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="DT1" s="4" t="s">
+      <c r="DT1" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="DU1" s="4" t="s">
+      <c r="DU1" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="DV1" s="4" t="s">
+      <c r="DV1" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="DW1" s="4" t="s">
+      <c r="DW1" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="DX1" s="4" t="s">
+      <c r="DX1" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="DY1" s="4" t="s">
+      <c r="DY1" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="DZ1" s="4" t="s">
+      <c r="DZ1" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="EA1" s="4" t="s">
+      <c r="EA1" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="EB1" s="4" t="s">
+      <c r="EB1" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="EC1" s="4" t="s">
+      <c r="EC1" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="ED1" s="4" t="s">
+      <c r="ED1" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="EE1" s="4" t="s">
+      <c r="EE1" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="EF1" s="4" t="s">
+      <c r="EF1" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="EG1" s="4" t="s">
+      <c r="EG1" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="EH1" s="4" t="s">
+      <c r="EH1" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="EI1" s="4" t="s">
+      <c r="EI1" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="EJ1" s="4" t="s">
+      <c r="EJ1" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="EK1" s="4" t="s">
+      <c r="EK1" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="EL1" s="4" t="s">
+      <c r="EL1" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="EM1" s="4" t="s">
+      <c r="EM1" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="EN1" s="4" t="s">
+      <c r="EN1" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="EO1" s="4" t="s">
+      <c r="EO1" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="EP1" s="4" t="s">
+      <c r="EP1" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="EQ1" s="4" t="s">
+      <c r="EQ1" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="ER1" s="4" t="s">
+      <c r="ER1" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="ES1" s="4" t="s">
+      <c r="ES1" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="ET1" s="4" t="s">
+      <c r="ET1" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="EU1" s="4" t="s">
+      <c r="EU1" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="EV1" s="4" t="s">
+      <c r="EV1" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="EW1" s="4" t="s">
+      <c r="EW1" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="EX1" s="4" t="s">
+      <c r="EX1" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="EY1" s="4" t="s">
+      <c r="EY1" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="EZ1" s="4" t="s">
+      <c r="EZ1" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="FA1" s="4" t="s">
+      <c r="FA1" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="FB1" s="4" t="s">
+      <c r="FB1" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="FC1" s="4" t="s">
+      <c r="FC1" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="FD1" s="4" t="s">
+      <c r="FD1" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="FE1" s="4" t="s">
+      <c r="FE1" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="FF1" s="4" t="s">
+      <c r="FF1" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="FG1" s="4" t="s">
+      <c r="FG1" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="FH1" s="4" t="s">
+      <c r="FH1" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="FI1" s="4" t="s">
+      <c r="FI1" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="FJ1" s="4" t="s">
+      <c r="FJ1" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="FK1" s="4" t="s">
+      <c r="FK1" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="FL1" s="4" t="s">
+      <c r="FL1" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="FM1" s="4" t="s">
+      <c r="FM1" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="FN1" s="4" t="s">
+      <c r="FN1" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="FO1" s="4" t="s">
+      <c r="FO1" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="FP1" s="4" t="s">
+      <c r="FP1" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="FQ1" s="4" t="s">
+      <c r="FQ1" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="FR1" s="4" t="s">
+      <c r="FR1" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="FS1" s="4" t="s">
+      <c r="FS1" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="FT1" s="4" t="s">
+      <c r="FT1" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="FU1" s="4" t="s">
+      <c r="FU1" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="FV1" s="4" t="s">
+      <c r="FV1" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="FW1" s="4" t="s">
+      <c r="FW1" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="FX1" s="4" t="s">
+      <c r="FX1" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="FY1" s="4" t="s">
+      <c r="FY1" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="FZ1" s="4" t="s">
+      <c r="FZ1" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="GA1" s="4" t="s">
+      <c r="GA1" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="GB1" s="4" t="s">
+      <c r="GB1" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="GC1" s="4" t="s">
+      <c r="GC1" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="GD1" s="4" t="s">
+      <c r="GD1" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="GE1" s="4" t="s">
+      <c r="GE1" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="GF1" s="4" t="s">
+      <c r="GF1" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="GG1" s="4" t="s">
+      <c r="GG1" s="2" t="s">
         <v>189</v>
       </c>
-      <c r="GH1" s="4" t="s">
+      <c r="GH1" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="GI1" s="4" t="s">
+      <c r="GI1" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="GJ1" s="4" t="s">
+      <c r="GJ1" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="GK1" s="4" t="s">
+      <c r="GK1" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="GL1" s="4" t="s">
+      <c r="GL1" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="GM1" s="4" t="s">
+      <c r="GM1" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="GN1" s="4" t="s">
+      <c r="GN1" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="GO1" s="4" t="s">
+      <c r="GO1" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="GP1" s="4" t="s">
+      <c r="GP1" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="GQ1" s="4" t="s">
+      <c r="GQ1" s="2" t="s">
         <v>199</v>
       </c>
-      <c r="GR1" s="4" t="s">
+      <c r="GR1" s="2" t="s">
         <v>200</v>
       </c>
-      <c r="GS1" s="4" t="s">
+      <c r="GS1" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="GT1" s="4" t="s">
+      <c r="GT1" s="2" t="s">
         <v>202</v>
       </c>
-      <c r="GU1" s="4" t="s">
+      <c r="GU1" s="2" t="s">
         <v>203</v>
       </c>
-      <c r="GV1" s="4" t="s">
+      <c r="GV1" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="GW1" s="4" t="s">
+      <c r="GW1" s="2" t="s">
         <v>205</v>
       </c>
-      <c r="GX1" s="4" t="s">
+      <c r="GX1" s="2" t="s">
         <v>206</v>
       </c>
-      <c r="GY1" s="4" t="s">
+      <c r="GY1" s="2" t="s">
         <v>207</v>
       </c>
-      <c r="GZ1" s="4" t="s">
+      <c r="GZ1" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="HA1" s="4" t="s">
+      <c r="HA1" s="2" t="s">
         <v>209</v>
       </c>
-      <c r="HB1" s="4" t="s">
+      <c r="HB1" s="2" t="s">
         <v>210</v>
       </c>
-      <c r="HC1" s="4" t="s">
+      <c r="HC1" s="2" t="s">
         <v>211</v>
       </c>
-      <c r="HD1" s="4" t="s">
+      <c r="HD1" s="2" t="s">
         <v>212</v>
       </c>
-      <c r="HE1" s="4" t="s">
+      <c r="HE1" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="HF1" s="4" t="s">
+      <c r="HF1" s="2" t="s">
         <v>214</v>
       </c>
-      <c r="HG1" s="4" t="s">
+      <c r="HG1" s="2" t="s">
         <v>215</v>
       </c>
-      <c r="HH1" s="4" t="s">
+      <c r="HH1" s="2" t="s">
         <v>216</v>
       </c>
-      <c r="HI1" s="4" t="s">
+      <c r="HI1" s="2" t="s">
         <v>217</v>
       </c>
-      <c r="HJ1" s="4" t="s">
+      <c r="HJ1" s="2" t="s">
         <v>218</v>
       </c>
-      <c r="HK1" s="4" t="s">
+      <c r="HK1" s="2" t="s">
         <v>219</v>
       </c>
-      <c r="HL1" s="4" t="s">
+      <c r="HL1" s="2" t="s">
         <v>220</v>
       </c>
-      <c r="HM1" s="4" t="s">
+      <c r="HM1" s="2" t="s">
         <v>221</v>
       </c>
-      <c r="HN1" s="4" t="s">
+      <c r="HN1" s="2" t="s">
         <v>222</v>
       </c>
-      <c r="HO1" s="4" t="s">
+      <c r="HO1" s="2" t="s">
         <v>223</v>
       </c>
-      <c r="HP1" s="4" t="s">
+      <c r="HP1" s="2" t="s">
         <v>224</v>
       </c>
-      <c r="HQ1" s="4" t="s">
+      <c r="HQ1" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="HR1" s="4" t="s">
+      <c r="HR1" s="2" t="s">
         <v>226</v>
       </c>
-      <c r="HS1" s="4" t="s">
+      <c r="HS1" s="2" t="s">
         <v>227</v>
       </c>
-      <c r="HT1" s="4" t="s">
+      <c r="HT1" s="2" t="s">
         <v>228</v>
       </c>
-      <c r="HU1" s="4" t="s">
+      <c r="HU1" s="2" t="s">
         <v>229</v>
       </c>
-      <c r="HV1" s="4" t="s">
+      <c r="HV1" s="2" t="s">
         <v>230</v>
       </c>
-      <c r="HW1" s="4" t="s">
+      <c r="HW1" s="2" t="s">
         <v>231</v>
       </c>
-      <c r="HX1" s="4" t="s">
+      <c r="HX1" s="2" t="s">
         <v>232</v>
       </c>
-      <c r="HY1" s="4" t="s">
+      <c r="HY1" s="2" t="s">
         <v>233</v>
       </c>
-      <c r="HZ1" s="4" t="s">
+      <c r="HZ1" s="2" t="s">
         <v>234</v>
       </c>
-      <c r="IA1" s="4" t="s">
+      <c r="IA1" s="2" t="s">
         <v>235</v>
       </c>
-      <c r="IB1" s="4" t="s">
+      <c r="IB1" s="2" t="s">
         <v>236</v>
       </c>
-      <c r="IC1" s="4" t="s">
+      <c r="IC1" s="2" t="s">
         <v>237</v>
       </c>
-      <c r="ID1" s="4" t="s">
+      <c r="ID1" s="2" t="s">
         <v>238</v>
       </c>
-      <c r="IE1" s="4" t="s">
+      <c r="IE1" s="2" t="s">
         <v>239</v>
       </c>
-      <c r="IF1" s="4" t="s">
+      <c r="IF1" s="2" t="s">
         <v>240</v>
       </c>
-      <c r="IG1" s="4" t="s">
+      <c r="IG1" s="2" t="s">
         <v>241</v>
       </c>
-      <c r="IH1" s="4" t="s">
+      <c r="IH1" s="2" t="s">
         <v>242</v>
       </c>
-      <c r="II1" s="4" t="s">
+      <c r="II1" s="2" t="s">
         <v>243</v>
       </c>
-      <c r="IJ1" s="4" t="s">
+      <c r="IJ1" s="2" t="s">
         <v>244</v>
       </c>
-      <c r="IK1" s="4" t="s">
+      <c r="IK1" s="2" t="s">
         <v>245</v>
       </c>
-      <c r="IL1" s="4" t="s">
+      <c r="IL1" s="2" t="s">
         <v>246</v>
       </c>
-      <c r="IM1" s="4" t="s">
+      <c r="IM1" s="2" t="s">
         <v>247</v>
       </c>
-      <c r="IN1" s="4" t="s">
+      <c r="IN1" s="2" t="s">
         <v>248</v>
       </c>
-      <c r="IO1" s="4" t="s">
+      <c r="IO1" s="2" t="s">
         <v>249</v>
       </c>
-      <c r="IP1" s="4" t="s">
+      <c r="IP1" s="2" t="s">
         <v>250</v>
       </c>
-      <c r="IQ1" s="4" t="s">
+      <c r="IQ1" s="2" t="s">
         <v>251</v>
       </c>
-      <c r="IR1" s="4" t="s">
+      <c r="IR1" s="2" t="s">
         <v>252</v>
       </c>
-      <c r="IS1" s="4" t="s">
+      <c r="IS1" s="2" t="s">
         <v>253</v>
       </c>
-      <c r="IT1" s="4" t="s">
+      <c r="IT1" s="2" t="s">
         <v>254</v>
       </c>
-      <c r="IU1" s="4" t="s">
+      <c r="IU1" s="2" t="s">
         <v>255</v>
       </c>
-      <c r="IV1" s="4" t="s">
+      <c r="IV1" s="2" t="s">
         <v>256</v>
       </c>
-      <c r="IW1" s="4" t="s">
+      <c r="IW1" s="2" t="s">
         <v>257</v>
       </c>
-      <c r="IX1" s="4" t="s">
+      <c r="IX1" s="2" t="s">
         <v>258</v>
       </c>
-      <c r="IY1" s="4" t="s">
+      <c r="IY1" s="2" t="s">
         <v>259</v>
       </c>
-      <c r="IZ1" s="4" t="s">
+      <c r="IZ1" s="2" t="s">
         <v>260</v>
       </c>
-      <c r="JA1" s="4" t="s">
+      <c r="JA1" s="2" t="s">
         <v>261</v>
       </c>
-      <c r="JB1" s="4" t="s">
+      <c r="JB1" s="2" t="s">
         <v>262</v>
       </c>
-      <c r="JC1" s="4" t="s">
+      <c r="JC1" s="2" t="s">
         <v>263</v>
       </c>
-      <c r="JD1" s="4" t="s">
+      <c r="JD1" s="2" t="s">
         <v>264</v>
       </c>
-      <c r="JE1" s="4" t="s">
+      <c r="JE1" s="2" t="s">
         <v>265</v>
       </c>
-      <c r="JF1" s="4" t="s">
+      <c r="JF1" s="2" t="s">
         <v>266</v>
       </c>
-      <c r="JG1" s="4" t="s">
+      <c r="JG1" s="2" t="s">
         <v>267</v>
       </c>
-      <c r="JH1" s="4" t="s">
+      <c r="JH1" s="2" t="s">
         <v>268</v>
       </c>
-      <c r="JI1" s="4" t="s">
+      <c r="JI1" s="2" t="s">
         <v>269</v>
       </c>
-      <c r="JJ1" s="4" t="s">
+      <c r="JJ1" s="2" t="s">
         <v>270</v>
       </c>
-      <c r="JK1" s="4" t="s">
+      <c r="JK1" s="2" t="s">
         <v>271</v>
       </c>
-      <c r="JL1" s="4" t="s">
+      <c r="JL1" s="2" t="s">
         <v>272</v>
       </c>
-      <c r="JM1" s="4" t="s">
+      <c r="JM1" s="2" t="s">
         <v>273</v>
       </c>
-      <c r="JN1" s="4" t="s">
+      <c r="JN1" s="2" t="s">
         <v>274</v>
       </c>
-      <c r="JO1" s="4" t="s">
+      <c r="JO1" s="2" t="s">
         <v>275</v>
       </c>
-      <c r="JP1" s="4" t="s">
+      <c r="JP1" s="2" t="s">
         <v>276</v>
       </c>
-      <c r="JQ1" s="4" t="s">
+      <c r="JQ1" s="2" t="s">
         <v>277</v>
       </c>
-      <c r="JR1" s="4" t="s">
+      <c r="JR1" s="2" t="s">
         <v>278</v>
       </c>
-      <c r="JS1" s="4" t="s">
+      <c r="JS1" s="2" t="s">
         <v>279</v>
       </c>
-      <c r="JT1" s="4" t="s">
+      <c r="JT1" s="2" t="s">
         <v>280</v>
       </c>
-      <c r="JU1" s="4" t="s">
+      <c r="JU1" s="2" t="s">
         <v>281</v>
       </c>
-      <c r="JV1" s="4" t="s">
+      <c r="JV1" s="2" t="s">
         <v>282</v>
       </c>
-      <c r="JW1" s="4" t="s">
+      <c r="JW1" s="2" t="s">
         <v>283</v>
       </c>
-      <c r="JX1" s="4" t="s">
+      <c r="JX1" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="JY1" s="4" t="s">
+      <c r="JY1" s="2" t="s">
         <v>285</v>
       </c>
-      <c r="JZ1" s="4" t="s">
+      <c r="JZ1" s="2" t="s">
         <v>286</v>
       </c>
-      <c r="KA1" s="4" t="s">
+      <c r="KA1" s="2" t="s">
         <v>287</v>
       </c>
-      <c r="KB1" s="4" t="s">
+      <c r="KB1" s="2" t="s">
         <v>288</v>
       </c>
-      <c r="KC1" s="4" t="s">
+      <c r="KC1" s="2" t="s">
         <v>289</v>
       </c>
-      <c r="KD1" s="4" t="s">
+      <c r="KD1" s="2" t="s">
         <v>290</v>
       </c>
-      <c r="KE1" s="4" t="s">
+      <c r="KE1" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="KF1" s="4" t="s">
+      <c r="KF1" s="2" t="s">
         <v>292</v>
       </c>
-      <c r="KG1" s="4" t="s">
+      <c r="KG1" s="2" t="s">
         <v>293</v>
       </c>
-      <c r="KH1" s="4" t="s">
+      <c r="KH1" s="2" t="s">
         <v>294</v>
       </c>
-      <c r="KI1" s="4" t="s">
+      <c r="KI1" s="2" t="s">
         <v>295</v>
       </c>
-      <c r="KJ1" s="4" t="s">
+      <c r="KJ1" s="2" t="s">
         <v>296</v>
       </c>
-      <c r="KK1" s="4" t="s">
+      <c r="KK1" s="2" t="s">
         <v>297</v>
       </c>
-      <c r="KL1" s="4" t="s">
+      <c r="KL1" s="2" t="s">
         <v>298</v>
       </c>
-      <c r="KM1" s="4" t="s">
+      <c r="KM1" s="2" t="s">
         <v>299</v>
       </c>
-      <c r="KN1" s="4" t="s">
+      <c r="KN1" s="2" t="s">
         <v>300</v>
       </c>
-      <c r="KO1" s="4" t="s">
+      <c r="KO1" s="2" t="s">
         <v>301</v>
       </c>
-      <c r="KP1" s="4" t="s">
+      <c r="KP1" s="2" t="s">
         <v>302</v>
       </c>
-      <c r="KQ1" s="4" t="s">
+      <c r="KQ1" s="2" t="s">
         <v>303</v>
       </c>
-      <c r="KR1" s="4" t="s">
+      <c r="KR1" s="2" t="s">
         <v>304</v>
       </c>
-      <c r="KS1" s="4" t="s">
+      <c r="KS1" s="2" t="s">
         <v>305</v>
       </c>
-      <c r="KT1" s="4" t="s">
+      <c r="KT1" s="2" t="s">
         <v>306</v>
       </c>
-      <c r="KU1" s="4" t="s">
+      <c r="KU1" s="2" t="s">
         <v>307</v>
       </c>
-      <c r="KV1" s="4" t="s">
+      <c r="KV1" s="2" t="s">
         <v>308</v>
       </c>
-      <c r="KW1" s="4" t="s">
+      <c r="KW1" s="2" t="s">
         <v>309</v>
       </c>
-      <c r="KX1" s="4" t="s">
+      <c r="KX1" s="2" t="s">
         <v>310</v>
       </c>
-      <c r="KY1" s="4" t="s">
+      <c r="KY1" s="2" t="s">
         <v>311</v>
       </c>
-      <c r="KZ1" s="4" t="s">
+      <c r="KZ1" s="2" t="s">
         <v>312</v>
       </c>
-      <c r="LA1" s="4" t="s">
+      <c r="LA1" s="2" t="s">
         <v>313</v>
       </c>
-      <c r="LB1" s="4" t="s">
+      <c r="LB1" s="2" t="s">
         <v>314</v>
       </c>
-      <c r="LC1" s="4" t="s">
+      <c r="LC1" s="2" t="s">
         <v>315</v>
       </c>
-      <c r="LD1" s="4" t="s">
+      <c r="LD1" s="2" t="s">
         <v>316</v>
       </c>
-      <c r="LE1" s="4" t="s">
+      <c r="LE1" s="2" t="s">
         <v>317</v>
       </c>
-      <c r="LF1" s="4" t="s">
+      <c r="LF1" s="2" t="s">
         <v>318</v>
       </c>
-      <c r="LG1" s="4" t="s">
+      <c r="LG1" s="2" t="s">
         <v>319</v>
       </c>
-      <c r="LH1" s="4" t="s">
+      <c r="LH1" s="2" t="s">
         <v>320</v>
       </c>
-      <c r="LI1" s="4" t="s">
+      <c r="LI1" s="2" t="s">
         <v>321</v>
       </c>
-      <c r="LJ1" s="4" t="s">
+      <c r="LJ1" s="2" t="s">
         <v>322</v>
       </c>
-      <c r="LK1" s="4" t="s">
+      <c r="LK1" s="2" t="s">
         <v>323</v>
       </c>
-      <c r="LL1" s="4" t="s">
+      <c r="LL1" s="2" t="s">
         <v>324</v>
       </c>
-      <c r="LM1" s="4" t="s">
+      <c r="LM1" s="2" t="s">
         <v>325</v>
       </c>
-      <c r="LN1" s="4" t="s">
+      <c r="LN1" s="2" t="s">
         <v>326</v>
       </c>
-      <c r="LO1" s="4" t="s">
+      <c r="LO1" s="2" t="s">
         <v>327</v>
       </c>
-      <c r="LP1" s="4" t="s">
+      <c r="LP1" s="2" t="s">
         <v>328</v>
       </c>
-      <c r="LQ1" s="4" t="s">
+      <c r="LQ1" s="2" t="s">
         <v>329</v>
       </c>
-      <c r="LR1" s="4" t="s">
+      <c r="LR1" s="2" t="s">
         <v>330</v>
       </c>
-      <c r="LS1" s="4" t="s">
+      <c r="LS1" s="2" t="s">
         <v>331</v>
       </c>
-      <c r="LT1" s="4" t="s">
+      <c r="LT1" s="2" t="s">
         <v>332</v>
       </c>
-      <c r="LU1" s="4" t="s">
+      <c r="LU1" s="2" t="s">
         <v>333</v>
       </c>
-      <c r="LV1" s="4" t="s">
+      <c r="LV1" s="2" t="s">
         <v>334</v>
       </c>
-      <c r="LW1" s="4" t="s">
+      <c r="LW1" s="2" t="s">
         <v>335</v>
       </c>
-      <c r="LX1" s="4" t="s">
+      <c r="LX1" s="2" t="s">
         <v>336</v>
       </c>
-      <c r="LY1" s="4" t="s">
+      <c r="LY1" s="2" t="s">
         <v>337</v>
       </c>
-      <c r="LZ1" s="4" t="s">
+      <c r="LZ1" s="2" t="s">
         <v>338</v>
       </c>
-      <c r="MA1" s="4" t="s">
+      <c r="MA1" s="2" t="s">
         <v>339</v>
       </c>
-      <c r="MB1" s="4" t="s">
+      <c r="MB1" s="2" t="s">
         <v>340</v>
       </c>
-      <c r="MC1" s="4" t="s">
+      <c r="MC1" s="2" t="s">
         <v>341</v>
       </c>
-      <c r="MD1" s="4" t="s">
+      <c r="MD1" s="2" t="s">
         <v>342</v>
       </c>
-      <c r="ME1" s="4" t="s">
+      <c r="ME1" s="2" t="s">
         <v>343</v>
       </c>
-      <c r="MF1" s="4" t="s">
+      <c r="MF1" s="2" t="s">
         <v>344</v>
       </c>
-      <c r="MG1" s="4" t="s">
+      <c r="MG1" s="2" t="s">
         <v>345</v>
       </c>
-      <c r="MH1" s="4" t="s">
+      <c r="MH1" s="2" t="s">
         <v>346</v>
       </c>
-      <c r="MI1" s="4" t="s">
+      <c r="MI1" s="2" t="s">
         <v>347</v>
       </c>
-      <c r="MJ1" s="4" t="s">
+      <c r="MJ1" s="2" t="s">
         <v>348</v>
       </c>
-      <c r="MK1" s="4" t="s">
+      <c r="MK1" s="2" t="s">
         <v>349</v>
       </c>
-      <c r="ML1" s="4" t="s">
+      <c r="ML1" s="2" t="s">
         <v>350</v>
       </c>
-      <c r="MM1" s="4" t="s">
+      <c r="MM1" s="2" t="s">
         <v>351</v>
       </c>
-      <c r="MN1" s="4" t="s">
+      <c r="MN1" s="2" t="s">
         <v>352</v>
       </c>
-      <c r="MO1" s="4" t="s">
+      <c r="MO1" s="2" t="s">
         <v>353</v>
       </c>
-      <c r="MP1" s="4" t="s">
+      <c r="MP1" s="2" t="s">
         <v>354</v>
       </c>
-      <c r="MQ1" s="4" t="s">
+      <c r="MQ1" s="2" t="s">
         <v>355</v>
       </c>
-      <c r="MR1" s="4" t="s">
+      <c r="MR1" s="2" t="s">
         <v>356</v>
       </c>
-      <c r="MS1" s="4" t="s">
+      <c r="MS1" s="2" t="s">
         <v>357</v>
       </c>
-      <c r="MT1" s="4" t="s">
+      <c r="MT1" s="2" t="s">
         <v>358</v>
       </c>
-      <c r="MU1" s="4" t="s">
+      <c r="MU1" s="2" t="s">
         <v>359</v>
       </c>
-      <c r="MV1" s="4" t="s">
+      <c r="MV1" s="2" t="s">
         <v>360</v>
       </c>
-      <c r="MW1" s="4" t="s">
+      <c r="MW1" s="2" t="s">
         <v>361</v>
       </c>
-      <c r="MX1" s="4" t="s">
+      <c r="MX1" s="2" t="s">
         <v>362</v>
       </c>
-      <c r="MY1" s="4" t="s">
+      <c r="MY1" s="2" t="s">
         <v>363</v>
       </c>
-      <c r="MZ1" s="4" t="s">
+      <c r="MZ1" s="2" t="s">
         <v>364</v>
       </c>
-      <c r="NA1" s="4" t="s">
+      <c r="NA1" s="2" t="s">
         <v>365</v>
       </c>
-      <c r="NB1" s="4" t="s">
+      <c r="NB1" s="2" t="s">
         <v>366</v>
       </c>
     </row>
@@ -9308,20 +9307,20 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="bfd95d43-064f-4848-903f-c1991b752d4e" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="bfd95d43-064f-4848-903f-c1991b752d4e" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -9564,14 +9563,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DC157F02-B06D-4B6E-B5BD-773BD056D0F5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CE3884A2-A688-4625-A5B7-97E6B309EBA6}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
@@ -9584,6 +9575,14 @@
     <ds:schemaRef ds:uri="bfd95d43-064f-4848-903f-c1991b752d4e"/>
     <ds:schemaRef ds:uri="19db16b9-8872-4c74-98c6-cce5390d2f7c"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DC157F02-B06D-4B6E-B5BD-773BD056D0F5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>